<commit_message>
Arquivo atualizado em 17/12/2023, 10:58:40.
</commit_message>
<xml_diff>
--- a/Data/g13.8.xlsx
+++ b/Data/g13.8.xlsx
@@ -1,46 +1,43 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
-  <workbookPr defaultThemeVersion="124226"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <workbookPr/>
+  <workbookProtection/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
+  <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="0"/>
   <fonts count="2">
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <color theme="1"/>
+      <sz val="11"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
+      <b val="1"/>
     </font>
   </fonts>
   <fills count="2">
     <fill>
-      <patternFill patternType="none"/>
+      <patternFill/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -48,21 +45,94 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="2">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
   </cellStyles>
-  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008000"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00808000"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="00C0C0C0"/>
+      <rgbColor rgb="00808080"/>
+      <rgbColor rgb="009999FF"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00FFFFCC"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00660066"/>
+      <rgbColor rgb="00FF8080"/>
+      <rgbColor rgb="000066CC"/>
+      <rgbColor rgb="00CCCCFF"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="0000CCFF"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00CCFFCC"/>
+      <rgbColor rgb="00FFFF99"/>
+      <rgbColor rgb="0099CCFF"/>
+      <rgbColor rgb="00FF99CC"/>
+      <rgbColor rgb="00CC99FF"/>
+      <rgbColor rgb="00FFCC99"/>
+      <rgbColor rgb="003366FF"/>
+      <rgbColor rgb="0033CCCC"/>
+      <rgbColor rgb="0099CC00"/>
+      <rgbColor rgb="00FFCC00"/>
+      <rgbColor rgb="00FF9900"/>
+      <rgbColor rgb="00FF6600"/>
+      <rgbColor rgb="00666699"/>
+      <rgbColor rgb="00969696"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
+    </indexedColors>
+  </colors>
 </styleSheet>
 </file>
 
@@ -350,14 +420,20 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D29"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:D45"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" s="1" customFormat="1">
+    <row r="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
           <t>Região</t>
@@ -365,17 +441,17 @@
       </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
-          <t>Variável</t>
+          <t>Ocupação</t>
         </is>
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
+          <t>Valor</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
           <t>Ano</t>
-        </is>
-      </c>
-      <c r="D1" s="1" t="inlineStr">
-        <is>
-          <t>Valor</t>
         </is>
       </c>
     </row>
@@ -387,16 +463,16 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Só estuda</t>
-        </is>
-      </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>31/12/2012</t>
-        </is>
-      </c>
-      <c r="D2">
-        <v>25.60534787983632</v>
+          <t>Estuda e está ocupado</t>
+        </is>
+      </c>
+      <c r="C2" t="n">
+        <v>11.96439345884951</v>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>01/01/2012</t>
+        </is>
       </c>
     </row>
     <row r="3">
@@ -407,16 +483,16 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>Só estuda</t>
-        </is>
-      </c>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>31/12/2017</t>
-        </is>
-      </c>
-      <c r="D3">
-        <v>24.63403429099106</v>
+          <t>Não estuda e não está ocupa</t>
+        </is>
+      </c>
+      <c r="C3" t="n">
+        <v>148.8451974099802</v>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>01/01/2012</t>
+        </is>
       </c>
     </row>
     <row r="4">
@@ -430,13 +506,13 @@
           <t>Só estuda</t>
         </is>
       </c>
-      <c r="C4" t="inlineStr">
-        <is>
-          <t>31/12/2018</t>
-        </is>
-      </c>
-      <c r="D4">
-        <v>28.40866137529308</v>
+      <c r="C4" t="n">
+        <v>25.60534787983632</v>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>01/01/2012</t>
+        </is>
       </c>
     </row>
     <row r="5">
@@ -447,16 +523,16 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>Só estuda</t>
-        </is>
-      </c>
-      <c r="C5" t="inlineStr">
-        <is>
-          <t>31/12/2019</t>
-        </is>
-      </c>
-      <c r="D5">
-        <v>26.09824277068888</v>
+          <t>Só está ocupado</t>
+        </is>
+      </c>
+      <c r="C5" t="n">
+        <v>38.2528652224094</v>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>01/01/2012</t>
+        </is>
       </c>
     </row>
     <row r="6">
@@ -467,16 +543,16 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>Só estuda</t>
-        </is>
-      </c>
-      <c r="C6" t="inlineStr">
-        <is>
-          <t>31/12/2020</t>
-        </is>
-      </c>
-      <c r="D6">
-        <v>29.6261672169715</v>
+          <t>Estuda e está ocupado</t>
+        </is>
+      </c>
+      <c r="C6" t="n">
+        <v>12.01231279225067</v>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>01/01/2013</t>
+        </is>
       </c>
     </row>
     <row r="7">
@@ -487,16 +563,16 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>Só estuda</t>
-        </is>
-      </c>
-      <c r="C7" t="inlineStr">
-        <is>
-          <t>31/12/2021</t>
-        </is>
-      </c>
-      <c r="D7">
-        <v>26.50874503070254</v>
+          <t>Não estuda e não está ocupa</t>
+        </is>
+      </c>
+      <c r="C7" t="n">
+        <v>151.6346608507999</v>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>01/01/2013</t>
+        </is>
       </c>
     </row>
     <row r="8">
@@ -510,13 +586,13 @@
           <t>Só estuda</t>
         </is>
       </c>
-      <c r="C8" t="inlineStr">
-        <is>
-          <t>31/12/2022</t>
-        </is>
-      </c>
-      <c r="D8">
-        <v>28.62124638481935</v>
+      <c r="C8" t="n">
+        <v>26.609715927658</v>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>01/01/2013</t>
+        </is>
       </c>
     </row>
     <row r="9">
@@ -527,16 +603,16 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>Estuda e trabalha</t>
-        </is>
-      </c>
-      <c r="C9" t="inlineStr">
-        <is>
-          <t>31/12/2012</t>
-        </is>
-      </c>
-      <c r="D9">
-        <v>11.96439345884951</v>
+          <t>Só está ocupado</t>
+        </is>
+      </c>
+      <c r="C9" t="n">
+        <v>36.90831472075404</v>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>01/01/2013</t>
+        </is>
       </c>
     </row>
     <row r="10">
@@ -547,16 +623,16 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>Estuda e trabalha</t>
-        </is>
-      </c>
-      <c r="C10" t="inlineStr">
-        <is>
-          <t>31/12/2017</t>
-        </is>
-      </c>
-      <c r="D10">
-        <v>9.678321003268797</v>
+          <t>Estuda e está ocupado</t>
+        </is>
+      </c>
+      <c r="C10" t="n">
+        <v>11.74810123988309</v>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>01/01/2014</t>
+        </is>
       </c>
     </row>
     <row r="11">
@@ -567,16 +643,16 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>Estuda e trabalha</t>
-        </is>
-      </c>
-      <c r="C11" t="inlineStr">
-        <is>
-          <t>31/12/2018</t>
-        </is>
-      </c>
-      <c r="D11">
-        <v>8.01773407447082</v>
+          <t>Não estuda e não está ocupa</t>
+        </is>
+      </c>
+      <c r="C11" t="n">
+        <v>142.03283628644</v>
+      </c>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>01/01/2014</t>
+        </is>
       </c>
     </row>
     <row r="12">
@@ -587,16 +663,16 @@
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>Estuda e trabalha</t>
-        </is>
-      </c>
-      <c r="C12" t="inlineStr">
-        <is>
-          <t>31/12/2019</t>
-        </is>
-      </c>
-      <c r="D12">
-        <v>8.97844527129217</v>
+          <t>Só estuda</t>
+        </is>
+      </c>
+      <c r="C12" t="n">
+        <v>24.87849391650491</v>
+      </c>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>01/01/2014</t>
+        </is>
       </c>
     </row>
     <row r="13">
@@ -607,16 +683,16 @@
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>Estuda e trabalha</t>
-        </is>
-      </c>
-      <c r="C13" t="inlineStr">
-        <is>
-          <t>31/12/2020</t>
-        </is>
-      </c>
-      <c r="D13">
-        <v>6.617084314546272</v>
+          <t>Só está ocupado</t>
+        </is>
+      </c>
+      <c r="C13" t="n">
+        <v>39.77447861099596</v>
+      </c>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t>01/01/2014</t>
+        </is>
       </c>
     </row>
     <row r="14">
@@ -627,16 +703,16 @@
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>Estuda e trabalha</t>
-        </is>
-      </c>
-      <c r="C14" t="inlineStr">
-        <is>
-          <t>31/12/2021</t>
-        </is>
-      </c>
-      <c r="D14">
-        <v>7.825615709242955</v>
+          <t>Estuda e está ocupado</t>
+        </is>
+      </c>
+      <c r="C14" t="n">
+        <v>10.88477532307686</v>
+      </c>
+      <c r="D14" t="inlineStr">
+        <is>
+          <t>01/01/2015</t>
+        </is>
       </c>
     </row>
     <row r="15">
@@ -647,16 +723,16 @@
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>Estuda e trabalha</t>
-        </is>
-      </c>
-      <c r="C15" t="inlineStr">
-        <is>
-          <t>31/12/2022</t>
-        </is>
-      </c>
-      <c r="D15">
-        <v>8.845564513098541</v>
+          <t>Não estuda e não está ocupa</t>
+        </is>
+      </c>
+      <c r="C15" t="n">
+        <v>154.3057717450601</v>
+      </c>
+      <c r="D15" t="inlineStr">
+        <is>
+          <t>01/01/2015</t>
+        </is>
       </c>
     </row>
     <row r="16">
@@ -667,16 +743,16 @@
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>Só trabalha</t>
-        </is>
-      </c>
-      <c r="C16" t="inlineStr">
-        <is>
-          <t>31/12/2012</t>
-        </is>
-      </c>
-      <c r="D16">
-        <v>38.2528652224094</v>
+          <t>Só estuda</t>
+        </is>
+      </c>
+      <c r="C16" t="n">
+        <v>25.64331488326894</v>
+      </c>
+      <c r="D16" t="inlineStr">
+        <is>
+          <t>01/01/2015</t>
+        </is>
       </c>
     </row>
     <row r="17">
@@ -687,16 +763,16 @@
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>Só trabalha</t>
-        </is>
-      </c>
-      <c r="C17" t="inlineStr">
-        <is>
-          <t>31/12/2017</t>
-        </is>
-      </c>
-      <c r="D17">
-        <v>35.04438297797804</v>
+          <t>Só está ocupado</t>
+        </is>
+      </c>
+      <c r="C17" t="n">
+        <v>37.98678297132652</v>
+      </c>
+      <c r="D17" t="inlineStr">
+        <is>
+          <t>01/01/2015</t>
+        </is>
       </c>
     </row>
     <row r="18">
@@ -707,16 +783,16 @@
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>Só trabalha</t>
-        </is>
-      </c>
-      <c r="C18" t="inlineStr">
-        <is>
-          <t>31/12/2018</t>
-        </is>
-      </c>
-      <c r="D18">
-        <v>32.27002225421842</v>
+          <t>Estuda e está ocupado</t>
+        </is>
+      </c>
+      <c r="C18" t="n">
+        <v>9.108069622139048</v>
+      </c>
+      <c r="D18" t="inlineStr">
+        <is>
+          <t>01/01/2016</t>
+        </is>
       </c>
     </row>
     <row r="19">
@@ -727,16 +803,16 @@
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>Só trabalha</t>
-        </is>
-      </c>
-      <c r="C19" t="inlineStr">
-        <is>
-          <t>31/12/2019</t>
-        </is>
-      </c>
-      <c r="D19">
-        <v>37.38420246533146</v>
+          <t>Não estuda e não está ocupa</t>
+        </is>
+      </c>
+      <c r="C19" t="n">
+        <v>166.7517624282901</v>
+      </c>
+      <c r="D19" t="inlineStr">
+        <is>
+          <t>01/01/2016</t>
+        </is>
       </c>
     </row>
     <row r="20">
@@ -747,16 +823,16 @@
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>Só trabalha</t>
-        </is>
-      </c>
-      <c r="C20" t="inlineStr">
-        <is>
-          <t>31/12/2020</t>
-        </is>
-      </c>
-      <c r="D20">
-        <v>31.3529002628708</v>
+          <t>Só estuda</t>
+        </is>
+      </c>
+      <c r="C20" t="n">
+        <v>25.77501322845462</v>
+      </c>
+      <c r="D20" t="inlineStr">
+        <is>
+          <t>01/01/2016</t>
+        </is>
       </c>
     </row>
     <row r="21">
@@ -767,16 +843,16 @@
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>Só trabalha</t>
-        </is>
-      </c>
-      <c r="C21" t="inlineStr">
-        <is>
-          <t>31/12/2021</t>
-        </is>
-      </c>
-      <c r="D21">
-        <v>32.69833830944476</v>
+          <t>Só está ocupado</t>
+        </is>
+      </c>
+      <c r="C21" t="n">
+        <v>37.41281354049283</v>
+      </c>
+      <c r="D21" t="inlineStr">
+        <is>
+          <t>01/01/2016</t>
+        </is>
       </c>
     </row>
     <row r="22">
@@ -787,16 +863,16 @@
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>Só trabalha</t>
-        </is>
-      </c>
-      <c r="C22" t="inlineStr">
-        <is>
-          <t>31/12/2022</t>
-        </is>
-      </c>
-      <c r="D22">
-        <v>35.35236730639497</v>
+          <t>Estuda e está ocupado</t>
+        </is>
+      </c>
+      <c r="C22" t="n">
+        <v>9.678321003268797</v>
+      </c>
+      <c r="D22" t="inlineStr">
+        <is>
+          <t>01/01/2017</t>
+        </is>
       </c>
     </row>
     <row r="23">
@@ -807,16 +883,16 @@
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>Não estuda e não trabalha</t>
-        </is>
-      </c>
-      <c r="C23" t="inlineStr">
-        <is>
-          <t>31/12/2012</t>
-        </is>
-      </c>
-      <c r="D23">
-        <v>24.17739343890454</v>
+          <t>Não estuda e não está ocupa</t>
+        </is>
+      </c>
+      <c r="C23" t="n">
+        <v>181.3020356201699</v>
+      </c>
+      <c r="D23" t="inlineStr">
+        <is>
+          <t>01/01/2017</t>
+        </is>
       </c>
     </row>
     <row r="24">
@@ -827,16 +903,16 @@
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>Não estuda e não trabalha</t>
-        </is>
-      </c>
-      <c r="C24" t="inlineStr">
-        <is>
-          <t>31/12/2017</t>
-        </is>
-      </c>
-      <c r="D24">
-        <v>30.6432617277623</v>
+          <t>Só estuda</t>
+        </is>
+      </c>
+      <c r="C24" t="n">
+        <v>24.63403429099106</v>
+      </c>
+      <c r="D24" t="inlineStr">
+        <is>
+          <t>01/01/2017</t>
+        </is>
       </c>
     </row>
     <row r="25">
@@ -847,16 +923,16 @@
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>Não estuda e não trabalha</t>
-        </is>
-      </c>
-      <c r="C25" t="inlineStr">
-        <is>
-          <t>31/12/2018</t>
-        </is>
-      </c>
-      <c r="D25">
-        <v>31.30358229601752</v>
+          <t>Só está ocupado</t>
+        </is>
+      </c>
+      <c r="C25" t="n">
+        <v>35.04438297797804</v>
+      </c>
+      <c r="D25" t="inlineStr">
+        <is>
+          <t>01/01/2017</t>
+        </is>
       </c>
     </row>
     <row r="26">
@@ -867,16 +943,16 @@
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>Não estuda e não trabalha</t>
-        </is>
-      </c>
-      <c r="C26" t="inlineStr">
-        <is>
-          <t>31/12/2019</t>
-        </is>
-      </c>
-      <c r="D26">
-        <v>27.53910949268759</v>
+          <t>Estuda e está ocupado</t>
+        </is>
+      </c>
+      <c r="C26" t="n">
+        <v>8.01773407447082</v>
+      </c>
+      <c r="D26" t="inlineStr">
+        <is>
+          <t>01/01/2018</t>
+        </is>
       </c>
     </row>
     <row r="27">
@@ -887,16 +963,16 @@
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>Não estuda e não trabalha</t>
-        </is>
-      </c>
-      <c r="C27" t="inlineStr">
-        <is>
-          <t>31/12/2020</t>
-        </is>
-      </c>
-      <c r="D27">
-        <v>32.40384820561173</v>
+          <t>Não estuda e não está ocupa</t>
+        </is>
+      </c>
+      <c r="C27" t="n">
+        <v>188.0478669516198</v>
+      </c>
+      <c r="D27" t="inlineStr">
+        <is>
+          <t>01/01/2018</t>
+        </is>
       </c>
     </row>
     <row r="28">
@@ -907,16 +983,16 @@
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>Não estuda e não trabalha</t>
-        </is>
-      </c>
-      <c r="C28" t="inlineStr">
-        <is>
-          <t>31/12/2021</t>
-        </is>
-      </c>
-      <c r="D28">
-        <v>32.96730095060988</v>
+          <t>Só estuda</t>
+        </is>
+      </c>
+      <c r="C28" t="n">
+        <v>28.40866137529308</v>
+      </c>
+      <c r="D28" t="inlineStr">
+        <is>
+          <t>01/01/2018</t>
+        </is>
       </c>
     </row>
     <row r="29">
@@ -927,19 +1003,339 @@
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>Não estuda e não trabalha</t>
-        </is>
-      </c>
-      <c r="C29" t="inlineStr">
-        <is>
-          <t>31/12/2022</t>
-        </is>
-      </c>
-      <c r="D29">
-        <v>27.18082179568723</v>
+          <t>Só está ocupado</t>
+        </is>
+      </c>
+      <c r="C29" t="n">
+        <v>32.27002225421842</v>
+      </c>
+      <c r="D29" t="inlineStr">
+        <is>
+          <t>01/01/2018</t>
+        </is>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="inlineStr">
+        <is>
+          <t>Sergipe</t>
+        </is>
+      </c>
+      <c r="B30" t="inlineStr">
+        <is>
+          <t>Estuda e está ocupado</t>
+        </is>
+      </c>
+      <c r="C30" t="n">
+        <v>8.97844527129217</v>
+      </c>
+      <c r="D30" t="inlineStr">
+        <is>
+          <t>01/01/2019</t>
+        </is>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="inlineStr">
+        <is>
+          <t>Sergipe</t>
+        </is>
+      </c>
+      <c r="B31" t="inlineStr">
+        <is>
+          <t>Não estuda e não está ocupa</t>
+        </is>
+      </c>
+      <c r="C31" t="n">
+        <v>169.52510976793</v>
+      </c>
+      <c r="D31" t="inlineStr">
+        <is>
+          <t>01/01/2019</t>
+        </is>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="inlineStr">
+        <is>
+          <t>Sergipe</t>
+        </is>
+      </c>
+      <c r="B32" t="inlineStr">
+        <is>
+          <t>Só estuda</t>
+        </is>
+      </c>
+      <c r="C32" t="n">
+        <v>26.09824277068884</v>
+      </c>
+      <c r="D32" t="inlineStr">
+        <is>
+          <t>01/01/2019</t>
+        </is>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="inlineStr">
+        <is>
+          <t>Sergipe</t>
+        </is>
+      </c>
+      <c r="B33" t="inlineStr">
+        <is>
+          <t>Só está ocupado</t>
+        </is>
+      </c>
+      <c r="C33" t="n">
+        <v>37.38420246533144</v>
+      </c>
+      <c r="D33" t="inlineStr">
+        <is>
+          <t>01/01/2019</t>
+        </is>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="inlineStr">
+        <is>
+          <t>Sergipe</t>
+        </is>
+      </c>
+      <c r="B34" t="inlineStr">
+        <is>
+          <t>Estuda e está ocupado</t>
+        </is>
+      </c>
+      <c r="C34" t="n">
+        <v>6.617084314546272</v>
+      </c>
+      <c r="D34" t="inlineStr">
+        <is>
+          <t>01/01/2020</t>
+        </is>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="inlineStr">
+        <is>
+          <t>Sergipe</t>
+        </is>
+      </c>
+      <c r="B35" t="inlineStr">
+        <is>
+          <t>Não estuda e não está ocupa</t>
+        </is>
+      </c>
+      <c r="C35" t="n">
+        <v>205.6669686557802</v>
+      </c>
+      <c r="D35" t="inlineStr">
+        <is>
+          <t>01/01/2020</t>
+        </is>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="inlineStr">
+        <is>
+          <t>Sergipe</t>
+        </is>
+      </c>
+      <c r="B36" t="inlineStr">
+        <is>
+          <t>Só estuda</t>
+        </is>
+      </c>
+      <c r="C36" t="n">
+        <v>29.6261672169715</v>
+      </c>
+      <c r="D36" t="inlineStr">
+        <is>
+          <t>01/01/2020</t>
+        </is>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="inlineStr">
+        <is>
+          <t>Sergipe</t>
+        </is>
+      </c>
+      <c r="B37" t="inlineStr">
+        <is>
+          <t>Só está ocupado</t>
+        </is>
+      </c>
+      <c r="C37" t="n">
+        <v>31.3529002628708</v>
+      </c>
+      <c r="D37" t="inlineStr">
+        <is>
+          <t>01/01/2020</t>
+        </is>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="inlineStr">
+        <is>
+          <t>Sergipe</t>
+        </is>
+      </c>
+      <c r="B38" t="inlineStr">
+        <is>
+          <t>Estuda e está ocupado</t>
+        </is>
+      </c>
+      <c r="C38" t="n">
+        <v>7.825615709242955</v>
+      </c>
+      <c r="D38" t="inlineStr">
+        <is>
+          <t>01/01/2021</t>
+        </is>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="inlineStr">
+        <is>
+          <t>Sergipe</t>
+        </is>
+      </c>
+      <c r="B39" t="inlineStr">
+        <is>
+          <t>Não estuda e não está ocupa</t>
+        </is>
+      </c>
+      <c r="C39" t="n">
+        <v>202.8693135388302</v>
+      </c>
+      <c r="D39" t="inlineStr">
+        <is>
+          <t>01/01/2021</t>
+        </is>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="inlineStr">
+        <is>
+          <t>Sergipe</t>
+        </is>
+      </c>
+      <c r="B40" t="inlineStr">
+        <is>
+          <t>Só estuda</t>
+        </is>
+      </c>
+      <c r="C40" t="n">
+        <v>26.50874503070254</v>
+      </c>
+      <c r="D40" t="inlineStr">
+        <is>
+          <t>01/01/2021</t>
+        </is>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="inlineStr">
+        <is>
+          <t>Sergipe</t>
+        </is>
+      </c>
+      <c r="B41" t="inlineStr">
+        <is>
+          <t>Só está ocupado</t>
+        </is>
+      </c>
+      <c r="C41" t="n">
+        <v>32.69833830944476</v>
+      </c>
+      <c r="D41" t="inlineStr">
+        <is>
+          <t>01/01/2021</t>
+        </is>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="inlineStr">
+        <is>
+          <t>Sergipe</t>
+        </is>
+      </c>
+      <c r="B42" t="inlineStr">
+        <is>
+          <t>Estuda e está ocupado</t>
+        </is>
+      </c>
+      <c r="C42" t="n">
+        <v>8.845564513098516</v>
+      </c>
+      <c r="D42" t="inlineStr">
+        <is>
+          <t>01/01/2022</t>
+        </is>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="inlineStr">
+        <is>
+          <t>Sergipe</t>
+        </is>
+      </c>
+      <c r="B43" t="inlineStr">
+        <is>
+          <t>Não estuda e não está ocupa</t>
+        </is>
+      </c>
+      <c r="C43" t="n">
+        <v>164.0409536947302</v>
+      </c>
+      <c r="D43" t="inlineStr">
+        <is>
+          <t>01/01/2022</t>
+        </is>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="inlineStr">
+        <is>
+          <t>Sergipe</t>
+        </is>
+      </c>
+      <c r="B44" t="inlineStr">
+        <is>
+          <t>Só estuda</t>
+        </is>
+      </c>
+      <c r="C44" t="n">
+        <v>28.62124638481927</v>
+      </c>
+      <c r="D44" t="inlineStr">
+        <is>
+          <t>01/01/2022</t>
+        </is>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" t="inlineStr">
+        <is>
+          <t>Sergipe</t>
+        </is>
+      </c>
+      <c r="B45" t="inlineStr">
+        <is>
+          <t>Só está ocupado</t>
+        </is>
+      </c>
+      <c r="C45" t="n">
+        <v>35.35236730639481</v>
+      </c>
+      <c r="D45" t="inlineStr">
+        <is>
+          <t>01/01/2022</t>
+        </is>
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
checkpoint g13; feito g13.8
</commit_message>
<xml_diff>
--- a/Data/g13.8.xlsx
+++ b/Data/g13.8.xlsx
@@ -1,46 +1,43 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
-  <workbookPr defaultThemeVersion="124226"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <workbookPr/>
+  <workbookProtection/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
+  <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="0"/>
   <fonts count="2">
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <color theme="1"/>
+      <sz val="11"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
+      <b val="1"/>
     </font>
   </fonts>
   <fills count="2">
     <fill>
-      <patternFill patternType="none"/>
+      <patternFill/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -48,21 +45,94 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="2">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
   </cellStyles>
-  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008000"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00808000"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="00C0C0C0"/>
+      <rgbColor rgb="00808080"/>
+      <rgbColor rgb="009999FF"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00FFFFCC"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00660066"/>
+      <rgbColor rgb="00FF8080"/>
+      <rgbColor rgb="000066CC"/>
+      <rgbColor rgb="00CCCCFF"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="0000CCFF"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00CCFFCC"/>
+      <rgbColor rgb="00FFFF99"/>
+      <rgbColor rgb="0099CCFF"/>
+      <rgbColor rgb="00FF99CC"/>
+      <rgbColor rgb="00CC99FF"/>
+      <rgbColor rgb="00FFCC99"/>
+      <rgbColor rgb="003366FF"/>
+      <rgbColor rgb="0033CCCC"/>
+      <rgbColor rgb="0099CC00"/>
+      <rgbColor rgb="00FFCC00"/>
+      <rgbColor rgb="00FF9900"/>
+      <rgbColor rgb="00FF6600"/>
+      <rgbColor rgb="00666699"/>
+      <rgbColor rgb="00969696"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
+    </indexedColors>
+  </colors>
 </styleSheet>
 </file>
 
@@ -350,14 +420,20 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
   <dimension ref="A1:D49"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" s="1" customFormat="1">
+    <row r="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
           <t>Região</t>
@@ -387,7 +463,7 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Só estuda</t>
+          <t>Estuda e trabalha</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
@@ -395,8 +471,8 @@
           <t>31/12/2012</t>
         </is>
       </c>
-      <c r="D2">
-        <v>25.60534787983632</v>
+      <c r="D2" t="n">
+        <v>11.96439345884951</v>
       </c>
     </row>
     <row r="3">
@@ -407,7 +483,7 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>Só estuda</t>
+          <t>Estuda e trabalha</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
@@ -415,8 +491,8 @@
           <t>31/12/2013</t>
         </is>
       </c>
-      <c r="D3">
-        <v>26.609715927658</v>
+      <c r="D3" t="n">
+        <v>12.01231279225067</v>
       </c>
     </row>
     <row r="4">
@@ -427,7 +503,7 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>Só estuda</t>
+          <t>Estuda e trabalha</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
@@ -435,8 +511,8 @@
           <t>31/12/2014</t>
         </is>
       </c>
-      <c r="D4">
-        <v>24.87849391650491</v>
+      <c r="D4" t="n">
+        <v>11.74810123988309</v>
       </c>
     </row>
     <row r="5">
@@ -447,7 +523,7 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>Só estuda</t>
+          <t>Estuda e trabalha</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
@@ -455,8 +531,8 @@
           <t>31/12/2015</t>
         </is>
       </c>
-      <c r="D5">
-        <v>25.6</v>
+      <c r="D5" t="n">
+        <v>10.88477532307686</v>
       </c>
     </row>
     <row r="6">
@@ -467,7 +543,7 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>Só estuda</t>
+          <t>Estuda e trabalha</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
@@ -475,8 +551,8 @@
           <t>31/12/2016</t>
         </is>
       </c>
-      <c r="D6">
-        <v>25.8</v>
+      <c r="D6" t="n">
+        <v>9.108069622139048</v>
       </c>
     </row>
     <row r="7">
@@ -487,7 +563,7 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>Só estuda</t>
+          <t>Estuda e trabalha</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
@@ -495,8 +571,8 @@
           <t>31/12/2017</t>
         </is>
       </c>
-      <c r="D7">
-        <v>24.63403429099106</v>
+      <c r="D7" t="n">
+        <v>9.678321003268797</v>
       </c>
     </row>
     <row r="8">
@@ -507,7 +583,7 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>Só estuda</t>
+          <t>Estuda e trabalha</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
@@ -515,8 +591,8 @@
           <t>31/12/2018</t>
         </is>
       </c>
-      <c r="D8">
-        <v>28.40866137529308</v>
+      <c r="D8" t="n">
+        <v>8.01773407447082</v>
       </c>
     </row>
     <row r="9">
@@ -527,7 +603,7 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>Só estuda</t>
+          <t>Estuda e trabalha</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
@@ -535,8 +611,8 @@
           <t>31/12/2019</t>
         </is>
       </c>
-      <c r="D9">
-        <v>26.09824277068888</v>
+      <c r="D9" t="n">
+        <v>8.97844527129217</v>
       </c>
     </row>
     <row r="10">
@@ -547,7 +623,7 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>Só estuda</t>
+          <t>Estuda e trabalha</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
@@ -555,8 +631,8 @@
           <t>31/12/2020</t>
         </is>
       </c>
-      <c r="D10">
-        <v>29.6261672169715</v>
+      <c r="D10" t="n">
+        <v>6.617084314546272</v>
       </c>
     </row>
     <row r="11">
@@ -567,7 +643,7 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>Só estuda</t>
+          <t>Estuda e trabalha</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
@@ -575,8 +651,8 @@
           <t>31/12/2021</t>
         </is>
       </c>
-      <c r="D11">
-        <v>26.50874503070254</v>
+      <c r="D11" t="n">
+        <v>7.825615709242955</v>
       </c>
     </row>
     <row r="12">
@@ -587,7 +663,7 @@
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>Só estuda</t>
+          <t>Estuda e trabalha</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
@@ -595,8 +671,8 @@
           <t>31/12/2022</t>
         </is>
       </c>
-      <c r="D12">
-        <v>28.62124638481935</v>
+      <c r="D12" t="n">
+        <v>8.845564513098513</v>
       </c>
     </row>
     <row r="13">
@@ -607,7 +683,7 @@
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>Só estuda</t>
+          <t>Estuda e trabalha</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
@@ -615,8 +691,8 @@
           <t>31/12/2023</t>
         </is>
       </c>
-      <c r="D13">
-        <v>26.6432472373036</v>
+      <c r="D13" t="n">
+        <v>9.163481684623161</v>
       </c>
     </row>
     <row r="14">
@@ -627,7 +703,7 @@
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>Estuda e trabalha</t>
+          <t>Não estuda e não trabalha</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
@@ -635,8 +711,8 @@
           <t>31/12/2012</t>
         </is>
       </c>
-      <c r="D14">
-        <v>11.96439345884951</v>
+      <c r="D14" t="n">
+        <v>24.17739343890454</v>
       </c>
     </row>
     <row r="15">
@@ -647,7 +723,7 @@
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>Estuda e trabalha</t>
+          <t>Não estuda e não trabalha</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
@@ -655,8 +731,8 @@
           <t>31/12/2013</t>
         </is>
       </c>
-      <c r="D15">
-        <v>12.01231279225067</v>
+      <c r="D15" t="n">
+        <v>24.46965655933733</v>
       </c>
     </row>
     <row r="16">
@@ -667,7 +743,7 @@
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>Estuda e trabalha</t>
+          <t>Não estuda e não trabalha</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
@@ -675,8 +751,8 @@
           <t>31/12/2014</t>
         </is>
       </c>
-      <c r="D16">
-        <v>11.74810123988309</v>
+      <c r="D16" t="n">
+        <v>23.59892623261636</v>
       </c>
     </row>
     <row r="17">
@@ -687,7 +763,7 @@
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>Estuda e trabalha</t>
+          <t>Não estuda e não trabalha</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
@@ -695,8 +771,8 @@
           <t>31/12/2015</t>
         </is>
       </c>
-      <c r="D17">
-        <v>10.9</v>
+      <c r="D17" t="n">
+        <v>25.48512682232793</v>
       </c>
     </row>
     <row r="18">
@@ -707,7 +783,7 @@
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>Estuda e trabalha</t>
+          <t>Não estuda e não trabalha</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
@@ -715,8 +791,8 @@
           <t>31/12/2016</t>
         </is>
       </c>
-      <c r="D18">
-        <v>9.1</v>
+      <c r="D18" t="n">
+        <v>27.70410360891397</v>
       </c>
     </row>
     <row r="19">
@@ -727,7 +803,7 @@
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>Estuda e trabalha</t>
+          <t>Não estuda e não trabalha</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
@@ -735,8 +811,8 @@
           <t>31/12/2017</t>
         </is>
       </c>
-      <c r="D19">
-        <v>9.678321003268797</v>
+      <c r="D19" t="n">
+        <v>30.6432617277623</v>
       </c>
     </row>
     <row r="20">
@@ -747,7 +823,7 @@
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>Estuda e trabalha</t>
+          <t>Não estuda e não trabalha</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
@@ -755,8 +831,8 @@
           <t>31/12/2018</t>
         </is>
       </c>
-      <c r="D20">
-        <v>8.01773407447082</v>
+      <c r="D20" t="n">
+        <v>31.30358229601752</v>
       </c>
     </row>
     <row r="21">
@@ -767,7 +843,7 @@
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>Estuda e trabalha</t>
+          <t>Não estuda e não trabalha</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
@@ -775,8 +851,8 @@
           <t>31/12/2019</t>
         </is>
       </c>
-      <c r="D21">
-        <v>8.97844527129217</v>
+      <c r="D21" t="n">
+        <v>27.53910949268757</v>
       </c>
     </row>
     <row r="22">
@@ -787,7 +863,7 @@
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>Estuda e trabalha</t>
+          <t>Não estuda e não trabalha</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
@@ -795,8 +871,8 @@
           <t>31/12/2020</t>
         </is>
       </c>
-      <c r="D22">
-        <v>6.617084314546272</v>
+      <c r="D22" t="n">
+        <v>32.40384820561173</v>
       </c>
     </row>
     <row r="23">
@@ -807,7 +883,7 @@
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>Estuda e trabalha</t>
+          <t>Não estuda e não trabalha</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
@@ -815,8 +891,8 @@
           <t>31/12/2021</t>
         </is>
       </c>
-      <c r="D23">
-        <v>7.825615709242955</v>
+      <c r="D23" t="n">
+        <v>32.96730095060988</v>
       </c>
     </row>
     <row r="24">
@@ -827,7 +903,7 @@
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>Estuda e trabalha</t>
+          <t>Não estuda e não trabalha</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
@@ -835,8 +911,8 @@
           <t>31/12/2022</t>
         </is>
       </c>
-      <c r="D24">
-        <v>8.845564513098541</v>
+      <c r="D24" t="n">
+        <v>27.18082179568713</v>
       </c>
     </row>
     <row r="25">
@@ -847,7 +923,7 @@
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>Estuda e trabalha</t>
+          <t>Não estuda e não trabalha</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
@@ -855,8 +931,8 @@
           <t>31/12/2023</t>
         </is>
       </c>
-      <c r="D25">
-        <v>9.163481684623161</v>
+      <c r="D25" t="n">
+        <v>27.01953231074691</v>
       </c>
     </row>
     <row r="26">
@@ -867,7 +943,7 @@
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>Só trabalha</t>
+          <t>Só estuda</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
@@ -875,8 +951,8 @@
           <t>31/12/2012</t>
         </is>
       </c>
-      <c r="D26">
-        <v>38.2528652224094</v>
+      <c r="D26" t="n">
+        <v>25.60534787983632</v>
       </c>
     </row>
     <row r="27">
@@ -887,7 +963,7 @@
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>Só trabalha</t>
+          <t>Só estuda</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
@@ -895,8 +971,8 @@
           <t>31/12/2013</t>
         </is>
       </c>
-      <c r="D27">
-        <v>36.90831472075404</v>
+      <c r="D27" t="n">
+        <v>26.609715927658</v>
       </c>
     </row>
     <row r="28">
@@ -907,7 +983,7 @@
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>Só trabalha</t>
+          <t>Só estuda</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
@@ -915,8 +991,8 @@
           <t>31/12/2014</t>
         </is>
       </c>
-      <c r="D28">
-        <v>39.77447861099596</v>
+      <c r="D28" t="n">
+        <v>24.87849391650491</v>
       </c>
     </row>
     <row r="29">
@@ -927,7 +1003,7 @@
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>Só trabalha</t>
+          <t>Só estuda</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
@@ -935,8 +1011,8 @@
           <t>31/12/2015</t>
         </is>
       </c>
-      <c r="D29">
-        <v>38</v>
+      <c r="D29" t="n">
+        <v>25.64331488326894</v>
       </c>
     </row>
     <row r="30">
@@ -947,7 +1023,7 @@
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>Só trabalha</t>
+          <t>Só estuda</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
@@ -955,8 +1031,8 @@
           <t>31/12/2016</t>
         </is>
       </c>
-      <c r="D30">
-        <v>37.4</v>
+      <c r="D30" t="n">
+        <v>25.77501322845462</v>
       </c>
     </row>
     <row r="31">
@@ -967,7 +1043,7 @@
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>Só trabalha</t>
+          <t>Só estuda</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
@@ -975,8 +1051,8 @@
           <t>31/12/2017</t>
         </is>
       </c>
-      <c r="D31">
-        <v>35.04438297797804</v>
+      <c r="D31" t="n">
+        <v>24.63403429099106</v>
       </c>
     </row>
     <row r="32">
@@ -987,7 +1063,7 @@
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>Só trabalha</t>
+          <t>Só estuda</t>
         </is>
       </c>
       <c r="C32" t="inlineStr">
@@ -995,8 +1071,8 @@
           <t>31/12/2018</t>
         </is>
       </c>
-      <c r="D32">
-        <v>32.27002225421842</v>
+      <c r="D32" t="n">
+        <v>28.40866137529308</v>
       </c>
     </row>
     <row r="33">
@@ -1007,7 +1083,7 @@
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>Só trabalha</t>
+          <t>Só estuda</t>
         </is>
       </c>
       <c r="C33" t="inlineStr">
@@ -1015,8 +1091,8 @@
           <t>31/12/2019</t>
         </is>
       </c>
-      <c r="D33">
-        <v>37.38420246533146</v>
+      <c r="D33" t="n">
+        <v>26.09824277068884</v>
       </c>
     </row>
     <row r="34">
@@ -1027,7 +1103,7 @@
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>Só trabalha</t>
+          <t>Só estuda</t>
         </is>
       </c>
       <c r="C34" t="inlineStr">
@@ -1035,8 +1111,8 @@
           <t>31/12/2020</t>
         </is>
       </c>
-      <c r="D34">
-        <v>31.3529002628708</v>
+      <c r="D34" t="n">
+        <v>29.6261672169715</v>
       </c>
     </row>
     <row r="35">
@@ -1047,7 +1123,7 @@
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>Só trabalha</t>
+          <t>Só estuda</t>
         </is>
       </c>
       <c r="C35" t="inlineStr">
@@ -1055,8 +1131,8 @@
           <t>31/12/2021</t>
         </is>
       </c>
-      <c r="D35">
-        <v>32.69833830944476</v>
+      <c r="D35" t="n">
+        <v>26.50874503070254</v>
       </c>
     </row>
     <row r="36">
@@ -1067,7 +1143,7 @@
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>Só trabalha</t>
+          <t>Só estuda</t>
         </is>
       </c>
       <c r="C36" t="inlineStr">
@@ -1075,8 +1151,8 @@
           <t>31/12/2022</t>
         </is>
       </c>
-      <c r="D36">
-        <v>35.35236730639497</v>
+      <c r="D36" t="n">
+        <v>28.62124638481926</v>
       </c>
     </row>
     <row r="37">
@@ -1087,7 +1163,7 @@
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>Só trabalha</t>
+          <t>Só estuda</t>
         </is>
       </c>
       <c r="C37" t="inlineStr">
@@ -1095,8 +1171,8 @@
           <t>31/12/2023</t>
         </is>
       </c>
-      <c r="D37">
-        <v>37.17373876732625</v>
+      <c r="D37" t="n">
+        <v>26.6432472373036</v>
       </c>
     </row>
     <row r="38">
@@ -1107,7 +1183,7 @@
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>Não estuda e não trabalha</t>
+          <t>Só trabalha</t>
         </is>
       </c>
       <c r="C38" t="inlineStr">
@@ -1115,8 +1191,8 @@
           <t>31/12/2012</t>
         </is>
       </c>
-      <c r="D38">
-        <v>24.17739343890454</v>
+      <c r="D38" t="n">
+        <v>38.2528652224094</v>
       </c>
     </row>
     <row r="39">
@@ -1127,7 +1203,7 @@
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>Não estuda e não trabalha</t>
+          <t>Só trabalha</t>
         </is>
       </c>
       <c r="C39" t="inlineStr">
@@ -1135,8 +1211,8 @@
           <t>31/12/2013</t>
         </is>
       </c>
-      <c r="D39">
-        <v>24.46965655933733</v>
+      <c r="D39" t="n">
+        <v>36.90831472075404</v>
       </c>
     </row>
     <row r="40">
@@ -1147,7 +1223,7 @@
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>Não estuda e não trabalha</t>
+          <t>Só trabalha</t>
         </is>
       </c>
       <c r="C40" t="inlineStr">
@@ -1155,8 +1231,8 @@
           <t>31/12/2014</t>
         </is>
       </c>
-      <c r="D40">
-        <v>23.59892623261636</v>
+      <c r="D40" t="n">
+        <v>39.77447861099596</v>
       </c>
     </row>
     <row r="41">
@@ -1167,7 +1243,7 @@
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>Não estuda e não trabalha</t>
+          <t>Só trabalha</t>
         </is>
       </c>
       <c r="C41" t="inlineStr">
@@ -1175,8 +1251,8 @@
           <t>31/12/2015</t>
         </is>
       </c>
-      <c r="D41">
-        <v>25.5</v>
+      <c r="D41" t="n">
+        <v>37.98678297132652</v>
       </c>
     </row>
     <row r="42">
@@ -1187,7 +1263,7 @@
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>Não estuda e não trabalha</t>
+          <t>Só trabalha</t>
         </is>
       </c>
       <c r="C42" t="inlineStr">
@@ -1195,8 +1271,8 @@
           <t>31/12/2016</t>
         </is>
       </c>
-      <c r="D42">
-        <v>27.7</v>
+      <c r="D42" t="n">
+        <v>37.41281354049283</v>
       </c>
     </row>
     <row r="43">
@@ -1207,7 +1283,7 @@
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>Não estuda e não trabalha</t>
+          <t>Só trabalha</t>
         </is>
       </c>
       <c r="C43" t="inlineStr">
@@ -1215,8 +1291,8 @@
           <t>31/12/2017</t>
         </is>
       </c>
-      <c r="D43">
-        <v>30.6432617277623</v>
+      <c r="D43" t="n">
+        <v>35.04438297797804</v>
       </c>
     </row>
     <row r="44">
@@ -1227,7 +1303,7 @@
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>Não estuda e não trabalha</t>
+          <t>Só trabalha</t>
         </is>
       </c>
       <c r="C44" t="inlineStr">
@@ -1235,8 +1311,8 @@
           <t>31/12/2018</t>
         </is>
       </c>
-      <c r="D44">
-        <v>31.30358229601752</v>
+      <c r="D44" t="n">
+        <v>32.27002225421842</v>
       </c>
     </row>
     <row r="45">
@@ -1247,7 +1323,7 @@
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>Não estuda e não trabalha</t>
+          <t>Só trabalha</t>
         </is>
       </c>
       <c r="C45" t="inlineStr">
@@ -1255,8 +1331,8 @@
           <t>31/12/2019</t>
         </is>
       </c>
-      <c r="D45">
-        <v>27.53910949268759</v>
+      <c r="D45" t="n">
+        <v>37.38420246533144</v>
       </c>
     </row>
     <row r="46">
@@ -1267,7 +1343,7 @@
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>Não estuda e não trabalha</t>
+          <t>Só trabalha</t>
         </is>
       </c>
       <c r="C46" t="inlineStr">
@@ -1275,8 +1351,8 @@
           <t>31/12/2020</t>
         </is>
       </c>
-      <c r="D46">
-        <v>32.40384820561173</v>
+      <c r="D46" t="n">
+        <v>31.3529002628708</v>
       </c>
     </row>
     <row r="47">
@@ -1287,7 +1363,7 @@
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>Não estuda e não trabalha</t>
+          <t>Só trabalha</t>
         </is>
       </c>
       <c r="C47" t="inlineStr">
@@ -1295,8 +1371,8 @@
           <t>31/12/2021</t>
         </is>
       </c>
-      <c r="D47">
-        <v>32.96730095060988</v>
+      <c r="D47" t="n">
+        <v>32.69833830944476</v>
       </c>
     </row>
     <row r="48">
@@ -1307,7 +1383,7 @@
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>Não estuda e não trabalha</t>
+          <t>Só trabalha</t>
         </is>
       </c>
       <c r="C48" t="inlineStr">
@@ -1315,8 +1391,8 @@
           <t>31/12/2022</t>
         </is>
       </c>
-      <c r="D48">
-        <v>27.18082179568723</v>
+      <c r="D48" t="n">
+        <v>35.3523673063948</v>
       </c>
     </row>
     <row r="49">
@@ -1327,7 +1403,7 @@
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>Não estuda e não trabalha</t>
+          <t>Só trabalha</t>
         </is>
       </c>
       <c r="C49" t="inlineStr">
@@ -1335,11 +1411,11 @@
           <t>31/12/2023</t>
         </is>
       </c>
-      <c r="D49">
-        <v>27.01953231074691</v>
+      <c r="D49" t="n">
+        <v>37.17373876732625</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
</xml_diff>